<commit_message>
Updated test exam again
</commit_message>
<xml_diff>
--- a/TestExam.xlsx
+++ b/TestExam.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maure\REPOSITORIES\OnlineExamCreator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2E63C6F-0E9F-4F29-A748-0A9D373C0961}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{095B4FE9-A1D3-4A80-8D50-4E672D5F9199}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General Information" sheetId="1" r:id="rId1"/>
@@ -57,9 +57,6 @@
     <t>Versions</t>
   </si>
   <si>
-    <t>Do. Or do not. There is no try.</t>
-  </si>
-  <si>
     <t>“In my experience there is no such thing as luck.”</t>
   </si>
   <si>
@@ -84,9 +81,6 @@
     <t>“A day may come when the courage of men fails… but it is not THIS day.”</t>
   </si>
   <si>
-    <t>"One Ring to rule them all, One Ring to find them, One Ring to bring them all and in the darkness bind them."</t>
-  </si>
-  <si>
     <t>"The doors of Durin, lord of Moria: Say 'friend' and enter."</t>
   </si>
   <si>
@@ -106,22 +100,20 @@
   </si>
   <si>
     <t>"I solemnly swear I am up to no good."</t>
+  </si>
+  <si>
+    <t>"Do. Or do not. There is no try."</t>
+  </si>
+  <si>
+    <t>"One Ring to rule them all, One Ring to find them, One Ring to bring them all and in the darkness bind them:"</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -149,12 +141,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -484,7 +472,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -511,27 +499,27 @@
         <v>25</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C3" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C4" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C5" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C6" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -543,8 +531,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7497C18A-E823-4D89-8B9F-96070B47D775}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -564,33 +552,33 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C2" s="2" t="s">
-        <v>18</v>
+      <c r="C2" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>
@@ -603,8 +591,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B40FC0E-889B-4E3E-97E0-ED46DC40F81E}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -624,33 +612,33 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C3" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C4" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C3" s="4" t="s">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C5" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C4" s="3" t="s">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C6" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C5" s="3" t="s">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C7" s="1" t="s">
         <v>23</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C6" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C7" s="3" t="s">
-        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Created route to show exams
</commit_message>
<xml_diff>
--- a/TestExam.xlsx
+++ b/TestExam.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maure\REPOSITORIES\OnlineExamCreator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{095B4FE9-A1D3-4A80-8D50-4E672D5F9199}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B9C05A7-9B6C-413D-802F-8A8B412B9058}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="General Information" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="30">
   <si>
     <t>Titel</t>
   </si>
@@ -48,9 +48,6 @@
     <t xml:space="preserve">Titel </t>
   </si>
   <si>
-    <t>Task 1</t>
-  </si>
-  <si>
     <t>Points</t>
   </si>
   <si>
@@ -106,6 +103,21 @@
   </si>
   <si>
     <t>"One Ring to rule them all, One Ring to find them, One Ring to bring them all and in the darkness bind them:"</t>
+  </si>
+  <si>
+    <t>Lord of the Rings</t>
+  </si>
+  <si>
+    <t>Star Wars</t>
+  </si>
+  <si>
+    <t>Harry Potter</t>
+  </si>
+  <si>
+    <t>Maurer</t>
+  </si>
+  <si>
+    <t>Project</t>
   </si>
 </sst>
 </file>
@@ -429,13 +441,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M28" sqref="M28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.140625" customWidth="1"/>
+    <col min="2" max="2" width="30.85546875" customWidth="1"/>
     <col min="3" max="3" width="12" customWidth="1"/>
     <col min="4" max="4" width="17.140625" customWidth="1"/>
   </cols>
@@ -455,6 +468,12 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" t="s">
+        <v>28</v>
+      </c>
       <c r="C2" t="s">
         <v>1</v>
       </c>
@@ -472,7 +491,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -485,41 +504,41 @@
         <v>5</v>
       </c>
       <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
         <v>7</v>
-      </c>
-      <c r="C1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>26</v>
       </c>
       <c r="B2">
         <v>25</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C3" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C4" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C5" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C6" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -531,12 +550,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7497C18A-E823-4D89-8B9F-96070B47D775}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="19.28515625" customWidth="1"/>
     <col min="3" max="3" width="98.85546875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -545,40 +565,46 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
         <v>7</v>
       </c>
-      <c r="C1" t="s">
-        <v>8</v>
-      </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2">
+        <v>30</v>
+      </c>
       <c r="C2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -592,7 +618,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -605,40 +631,46 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
         <v>7</v>
       </c>
-      <c r="C1" t="s">
-        <v>8</v>
-      </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B2">
+        <v>45</v>
+      </c>
       <c r="C2" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C3" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C4" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C5" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C6" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C7" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>